<commit_message>
changed BOM & resistor values. Sent to accutrace for assy.
</commit_message>
<xml_diff>
--- a/Drumpants_A1_BOM_rev2.xlsx
+++ b/Drumpants_A1_BOM_rev2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="22056" yWindow="-96" windowWidth="22980" windowHeight="11556"/>
+    <workbookView xWindow="22050" yWindow="-90" windowWidth="22980" windowHeight="11550"/>
   </bookViews>
   <sheets>
     <sheet name="BOARD" sheetId="1" r:id="rId1"/>
     <sheet name="BREAKOUT" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -870,11 +870,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1719,7 +1719,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2028,7 +2028,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -2308,6 +2308,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -2342,6 +2343,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2517,44 +2519,44 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+      <selection activeCell="D32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="110.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.109375" style="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="121" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.140625" style="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22" style="12" customWidth="1"/>
-    <col min="5" max="5" width="19.44140625" style="12" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" style="12" customWidth="1"/>
     <col min="6" max="6" width="28" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" style="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="30" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.88671875" style="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.5546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" style="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" style="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.5703125" style="12" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="28" style="12" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.44140625" style="24" customWidth="1"/>
-    <col min="20" max="20" width="18.88671875" style="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" style="24" customWidth="1"/>
+    <col min="20" max="20" width="18.85546875" style="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="26" style="12" customWidth="1"/>
-    <col min="22" max="22" width="13.44140625" style="12" customWidth="1"/>
-    <col min="23" max="23" width="11.6640625" style="12" customWidth="1"/>
-    <col min="24" max="24" width="17.44140625" style="12" customWidth="1"/>
-    <col min="25" max="25" width="17.109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="12"/>
+    <col min="22" max="22" width="13.42578125" style="12" customWidth="1"/>
+    <col min="23" max="23" width="11.7109375" style="12" customWidth="1"/>
+    <col min="24" max="24" width="17.42578125" style="12" customWidth="1"/>
+    <col min="25" max="25" width="17.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.140625" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="11" customFormat="1">
+    <row r="1" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -2628,7 +2630,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>253</v>
       </c>
@@ -2698,7 +2700,7 @@
       </c>
       <c r="Y2" s="12"/>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>25</v>
       </c>
@@ -2768,7 +2770,7 @@
       </c>
       <c r="Y3" s="12"/>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>65</v>
       </c>
@@ -2838,7 +2840,7 @@
       </c>
       <c r="Y4" s="12"/>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
         <v>254</v>
       </c>
@@ -2908,7 +2910,7 @@
       </c>
       <c r="Y5" s="12"/>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>258</v>
       </c>
@@ -2978,7 +2980,7 @@
       </c>
       <c r="Y6" s="12"/>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
         <v>20</v>
       </c>
@@ -3048,7 +3050,7 @@
       </c>
       <c r="Y7" s="12"/>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
         <v>17</v>
       </c>
@@ -3118,7 +3120,7 @@
       </c>
       <c r="Y8" s="12"/>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>57</v>
       </c>
@@ -3188,7 +3190,7 @@
       </c>
       <c r="Y9" s="12"/>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>48</v>
       </c>
@@ -3258,7 +3260,7 @@
       </c>
       <c r="Y10" s="12"/>
     </row>
-    <row r="11" spans="1:25" ht="15" customHeight="1">
+    <row r="11" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>67</v>
       </c>
@@ -3328,7 +3330,7 @@
       </c>
       <c r="Y11" s="12"/>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>44</v>
       </c>
@@ -3400,7 +3402,7 @@
       </c>
       <c r="Y12" s="12"/>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>255</v>
       </c>
@@ -3470,7 +3472,7 @@
       </c>
       <c r="Y13" s="12"/>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>256</v>
       </c>
@@ -3540,7 +3542,7 @@
       </c>
       <c r="Y14" s="12"/>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
         <v>14</v>
       </c>
@@ -3610,7 +3612,7 @@
       </c>
       <c r="Y15" s="12"/>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
         <v>22</v>
       </c>
@@ -3680,7 +3682,7 @@
       </c>
       <c r="Y16" s="12"/>
     </row>
-    <row r="17" spans="1:25">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A17" s="18" t="s">
         <v>56</v>
       </c>
@@ -3750,7 +3752,7 @@
       </c>
       <c r="Y17" s="12"/>
     </row>
-    <row r="18" spans="1:25">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
         <v>63</v>
       </c>
@@ -3820,7 +3822,7 @@
       </c>
       <c r="Y18" s="12"/>
     </row>
-    <row r="19" spans="1:25">
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A19" s="18" t="s">
         <v>257</v>
       </c>
@@ -3890,7 +3892,7 @@
       </c>
       <c r="Y19" s="12"/>
     </row>
-    <row r="20" spans="1:25">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
         <v>6</v>
       </c>
@@ -3960,7 +3962,7 @@
       </c>
       <c r="Y20" s="12"/>
     </row>
-    <row r="21" spans="1:25">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" s="18" t="s">
         <v>99</v>
       </c>
@@ -4030,7 +4032,7 @@
       </c>
       <c r="Y21" s="12"/>
     </row>
-    <row r="22" spans="1:25">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
         <v>41</v>
       </c>
@@ -4100,7 +4102,7 @@
       </c>
       <c r="Y22" s="12"/>
     </row>
-    <row r="23" spans="1:25">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" s="18" t="s">
         <v>91</v>
       </c>
@@ -4170,7 +4172,7 @@
       </c>
       <c r="Y23" s="12"/>
     </row>
-    <row r="24" spans="1:25">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
         <v>94</v>
       </c>
@@ -4240,7 +4242,7 @@
       </c>
       <c r="Y24" s="12"/>
     </row>
-    <row r="25" spans="1:25">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A25" s="18" t="s">
         <v>180</v>
       </c>
@@ -4309,7 +4311,7 @@
       </c>
       <c r="Y25" s="12"/>
     </row>
-    <row r="26" spans="1:25">
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A26" s="18" t="s">
         <v>76</v>
       </c>
@@ -4379,7 +4381,7 @@
       </c>
       <c r="Y26" s="12"/>
     </row>
-    <row r="27" spans="1:25">
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>89</v>
       </c>
@@ -4449,7 +4451,7 @@
       </c>
       <c r="Y27" s="12"/>
     </row>
-    <row r="28" spans="1:25">
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
         <v>34</v>
       </c>
@@ -4519,7 +4521,7 @@
       </c>
       <c r="Y28" s="12"/>
     </row>
-    <row r="29" spans="1:25" ht="13.95" customHeight="1">
+    <row r="29" spans="1:25" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18" t="s">
         <v>24</v>
       </c>
@@ -4589,7 +4591,7 @@
       </c>
       <c r="Y29" s="12"/>
     </row>
-    <row r="30" spans="1:25">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A30" s="18" t="s">
         <v>12</v>
       </c>
@@ -4659,7 +4661,7 @@
       </c>
       <c r="Y30" s="12"/>
     </row>
-    <row r="31" spans="1:25">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
         <v>68</v>
       </c>
@@ -4729,7 +4731,7 @@
       </c>
       <c r="Y31" s="12"/>
     </row>
-    <row r="32" spans="1:25">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>45</v>
       </c>
@@ -4799,7 +4801,7 @@
       </c>
       <c r="Y32" s="12"/>
     </row>
-    <row r="33" spans="1:25">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A33" s="18" t="s">
         <v>73</v>
       </c>
@@ -4869,7 +4871,7 @@
       </c>
       <c r="Y33" s="12"/>
     </row>
-    <row r="34" spans="1:25">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A34" s="18" t="s">
         <v>81</v>
       </c>
@@ -4939,7 +4941,7 @@
       </c>
       <c r="Y34" s="12"/>
     </row>
-    <row r="35" spans="1:25">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>70</v>
       </c>
@@ -5009,7 +5011,7 @@
       </c>
       <c r="Y35" s="12"/>
     </row>
-    <row r="36" spans="1:25">
+    <row r="36" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A36" s="18" t="s">
         <v>97</v>
       </c>
@@ -5079,7 +5081,7 @@
       </c>
       <c r="Y36" s="12"/>
     </row>
-    <row r="37" spans="1:25">
+    <row r="37" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A37" s="18" t="s">
         <v>50</v>
       </c>
@@ -5149,7 +5151,7 @@
       </c>
       <c r="Y37" s="12"/>
     </row>
-    <row r="38" spans="1:25">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A38" s="18" t="s">
         <v>5</v>
       </c>
@@ -5221,7 +5223,7 @@
       </c>
       <c r="Y38" s="12"/>
     </row>
-    <row r="39" spans="1:25">
+    <row r="39" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A39" s="18" t="s">
         <v>52</v>
       </c>
@@ -5291,7 +5293,7 @@
       </c>
       <c r="Y39" s="12"/>
     </row>
-    <row r="40" spans="1:25">
+    <row r="40" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A40" s="18" t="s">
         <v>59</v>
       </c>
@@ -5361,7 +5363,7 @@
       </c>
       <c r="Y40" s="12"/>
     </row>
-    <row r="41" spans="1:25">
+    <row r="41" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A41" s="18" t="s">
         <v>62</v>
       </c>
@@ -5431,7 +5433,7 @@
       </c>
       <c r="Y41" s="12"/>
     </row>
-    <row r="42" spans="1:25">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A42" s="18" t="s">
         <v>78</v>
       </c>
@@ -5501,7 +5503,7 @@
       </c>
       <c r="Y42" s="12"/>
     </row>
-    <row r="43" spans="1:25">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A43" s="18" t="s">
         <v>36</v>
       </c>
@@ -5571,7 +5573,7 @@
       </c>
       <c r="Y43" s="12"/>
     </row>
-    <row r="44" spans="1:25">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
         <v>84</v>
       </c>
@@ -5641,7 +5643,7 @@
       </c>
       <c r="Y44" s="12"/>
     </row>
-    <row r="45" spans="1:25">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A45" s="18" t="s">
         <v>87</v>
       </c>
@@ -5711,7 +5713,7 @@
       </c>
       <c r="Y45" s="12"/>
     </row>
-    <row r="46" spans="1:25">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A46" s="18" t="s">
         <v>259</v>
       </c>
@@ -5779,7 +5781,7 @@
       </c>
       <c r="Y46" s="12"/>
     </row>
-    <row r="47" spans="1:25">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A47" s="20" t="s">
         <v>30</v>
       </c>
@@ -5847,7 +5849,7 @@
       </c>
       <c r="Y47" s="12"/>
     </row>
-    <row r="48" spans="1:25" customFormat="1">
+    <row r="48" spans="1:25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="18" t="s">
         <v>38</v>
       </c>
@@ -5914,7 +5916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:25">
+    <row r="49" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>55</v>
       </c>
@@ -5982,7 +5984,7 @@
       </c>
       <c r="Y49" s="12"/>
     </row>
-    <row r="50" spans="1:25">
+    <row r="50" spans="1:25" x14ac:dyDescent="0.25">
       <c r="X50" s="13">
         <f>SUM(Table1[Cheapest Price])</f>
         <v>21591.15</v>
@@ -6023,16 +6025,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" s="12" customFormat="1">
+    <row r="1" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="18" t="s">
         <v>27</v>
       </c>
@@ -6101,7 +6103,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="2" spans="1:24" s="12" customFormat="1">
+    <row r="2" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>34</v>
       </c>

</xml_diff>